<commit_message>
atualizando teste da pagina fundamental
</commit_message>
<xml_diff>
--- a/Segundo passo/Componente fundamental.xlsx
+++ b/Segundo passo/Componente fundamental.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DTI DIGITAL\Desktop\DTI Digital\roteirosDeTeste\Segundo passo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{352654F0-CA5C-4444-B9C4-7DFF9900C9D3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEF9A5DC-0071-4C0A-B34B-A741D3A17311}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Checklist Flow" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="154">
   <si>
     <t>CHECKLIST FLOW</t>
   </si>
@@ -479,6 +479,30 @@
   </si>
   <si>
     <t>Ao passar do passo 1 para o passo 2, enquanto esse processo é feito, deve aparecer um modal com loading informando o carregamento da pág.</t>
+  </si>
+  <si>
+    <t>1.4</t>
+  </si>
+  <si>
+    <t>1.5</t>
+  </si>
+  <si>
+    <t>1.6</t>
+  </si>
+  <si>
+    <t>1.7</t>
+  </si>
+  <si>
+    <t>1.8</t>
+  </si>
+  <si>
+    <t>1.9</t>
+  </si>
+  <si>
+    <t>Conexão entre passo 1 e passo 2</t>
+  </si>
+  <si>
+    <t>Apos preencher todos os campos do passo 1, ao clicar no button, deve passar para  o passo 2 com os grupos de carros referente a agência de retirada escolhida.</t>
   </si>
 </sst>
 </file>
@@ -1415,10 +1439,19 @@
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1524,15 +1557,6 @@
     </xf>
     <xf numFmtId="164" fontId="3" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -11174,12 +11198,12 @@
     <row r="1" spans="2:18" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:18" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:18" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
     </row>
     <row r="4" spans="2:18" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
@@ -11416,10 +11440,10 @@
   <sheetPr>
     <tabColor rgb="FF376092"/>
   </sheetPr>
-  <dimension ref="A2:AMK29"/>
+  <dimension ref="A2:AMK31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -11435,16 +11459,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="78" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="75"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="76" t="s">
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="79" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="10"/>
@@ -11460,17 +11484,17 @@
       <c r="A4" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="73" t="s">
+      <c r="B4" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="73"/>
+      <c r="C4" s="75"/>
       <c r="D4" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="74" t="s">
+      <c r="E4" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="74"/>
+      <c r="F4" s="77"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
@@ -11517,7 +11541,7 @@
       <c r="B7" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="C7" s="109" t="s">
+      <c r="C7" s="72" t="s">
         <v>136</v>
       </c>
       <c r="D7" s="15"/>
@@ -11535,7 +11559,7 @@
       <c r="B8" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="C8" s="109" t="s">
+      <c r="C8" s="72" t="s">
         <v>138</v>
       </c>
       <c r="D8" s="15"/>
@@ -11566,12 +11590,12 @@
     </row>
     <row r="10" spans="1:6" ht="45" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" s="110" t="s">
+        <v>146</v>
+      </c>
+      <c r="B10" s="73" t="s">
         <v>139</v>
       </c>
-      <c r="C10" s="109" t="s">
+      <c r="C10" s="72" t="s">
         <v>141</v>
       </c>
       <c r="D10" s="15"/>
@@ -11584,7 +11608,7 @@
     </row>
     <row r="11" spans="1:6" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>35</v>
+        <v>147</v>
       </c>
       <c r="B11" s="14" t="s">
         <v>132</v>
@@ -11601,7 +11625,9 @@
       </c>
     </row>
     <row r="12" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
+      <c r="A12" s="13" t="s">
+        <v>148</v>
+      </c>
       <c r="B12" s="14" t="s">
         <v>142</v>
       </c>
@@ -11618,7 +11644,7 @@
     </row>
     <row r="13" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>34</v>
+        <v>149</v>
       </c>
       <c r="B13" s="14" t="s">
         <v>134</v>
@@ -11627,88 +11653,82 @@
         <v>143</v>
       </c>
       <c r="D13" s="15"/>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+    </row>
+    <row r="14" spans="1:6" ht="60" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="D14" s="15"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+    </row>
+    <row r="15" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="D15" s="15"/>
+      <c r="E15" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F15" s="16" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-    </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="73" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="108"/>
-      <c r="D15" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15" s="74" t="s">
-        <v>24</v>
-      </c>
-      <c r="F15" s="74"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="12">
-        <v>2</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="F16" s="12" t="s">
-        <v>31</v>
-      </c>
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="16" t="s">
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="75" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="76"/>
+      <c r="D17" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="F17" s="77"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="F18" s="16" t="s">
-        <v>24</v>
+      <c r="A18" s="12">
+        <v>2</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
@@ -11722,7 +11742,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B20" s="14"/>
       <c r="C20" s="14"/>
@@ -11736,7 +11756,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B21" s="14"/>
       <c r="C21" s="14"/>
@@ -11750,7 +11770,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B22" s="14"/>
       <c r="C22" s="14"/>
@@ -11764,7 +11784,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B23" s="14"/>
       <c r="C23" s="14"/>
@@ -11776,73 +11796,73 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="F25" s="16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="73" t="s">
+      <c r="B27" s="75" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="108"/>
-      <c r="D25" s="11" t="s">
+      <c r="C27" s="76"/>
+      <c r="D27" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E25" s="74" t="s">
+      <c r="E27" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="F25" s="74"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="12">
-        <v>3</v>
-      </c>
-      <c r="B26" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="D26" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="E26" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="F26" s="12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="F27" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="F27" s="77"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="B28" s="14"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="F28" s="16" t="s">
-        <v>24</v>
+      <c r="A28" s="12">
+        <v>3</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B29" s="14"/>
       <c r="C29" s="14"/>
@@ -11854,18 +11874,46 @@
         <v>24</v>
       </c>
     </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="F30" s="16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31" s="14"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="F31" s="16" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="E27:F27"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="E4:F4"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="E17:F17"/>
   </mergeCells>
-  <conditionalFormatting sqref="D2 E10:F12">
+  <conditionalFormatting sqref="D2 E10:F14">
     <cfRule type="cellIs" dxfId="351" priority="2" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -11887,7 +11935,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E7:F7 E10:F12">
+  <conditionalFormatting sqref="E7:F7 E10:F14">
     <cfRule type="cellIs" dxfId="345" priority="8" operator="equal">
       <formula>"Concluído"</formula>
     </cfRule>
@@ -11898,7 +11946,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E7:F7 E10:F12">
+  <conditionalFormatting sqref="E7:F7 E10:F14">
     <cfRule type="cellIs" dxfId="342" priority="11" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -11942,7 +11990,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E13:F13">
+  <conditionalFormatting sqref="E15:F15">
     <cfRule type="cellIs" dxfId="330" priority="23" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -11953,7 +12001,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E13:F13">
+  <conditionalFormatting sqref="E15:F15">
     <cfRule type="cellIs" dxfId="327" priority="26" operator="equal">
       <formula>"Concluído"</formula>
     </cfRule>
@@ -11964,7 +12012,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E13:F13">
+  <conditionalFormatting sqref="E15:F15">
     <cfRule type="cellIs" dxfId="324" priority="29" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -11975,7 +12023,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E13">
+  <conditionalFormatting sqref="E15">
     <cfRule type="cellIs" dxfId="321" priority="32" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -11986,7 +12034,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E13">
+  <conditionalFormatting sqref="E15">
     <cfRule type="cellIs" dxfId="318" priority="35" operator="equal">
       <formula>"Concluído"</formula>
     </cfRule>
@@ -11997,7 +12045,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E13">
+  <conditionalFormatting sqref="E15">
     <cfRule type="cellIs" dxfId="315" priority="38" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -12008,7 +12056,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F13">
+  <conditionalFormatting sqref="F15">
     <cfRule type="cellIs" dxfId="312" priority="41" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -12019,7 +12067,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F13">
+  <conditionalFormatting sqref="F15">
     <cfRule type="cellIs" dxfId="309" priority="44" operator="equal">
       <formula>"Concluído"</formula>
     </cfRule>
@@ -12030,7 +12078,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F13">
+  <conditionalFormatting sqref="F15">
     <cfRule type="cellIs" dxfId="306" priority="47" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -12239,7 +12287,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E15 E18:F18">
+  <conditionalFormatting sqref="E17 E20:F20">
     <cfRule type="cellIs" dxfId="249" priority="122" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -12250,7 +12298,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E18:F18">
+  <conditionalFormatting sqref="E20:F20">
     <cfRule type="cellIs" dxfId="246" priority="125" operator="equal">
       <formula>"Concluído"</formula>
     </cfRule>
@@ -12261,7 +12309,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E18:F18">
+  <conditionalFormatting sqref="E20:F20">
     <cfRule type="cellIs" dxfId="243" priority="128" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -12272,7 +12320,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E17:F18">
+  <conditionalFormatting sqref="E19:F20">
     <cfRule type="cellIs" dxfId="240" priority="131" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -12283,7 +12331,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E17:F18">
+  <conditionalFormatting sqref="E19:F20">
     <cfRule type="cellIs" dxfId="237" priority="134" operator="equal">
       <formula>"Concluído"</formula>
     </cfRule>
@@ -12294,7 +12342,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E17:F18">
+  <conditionalFormatting sqref="E19:F20">
     <cfRule type="cellIs" dxfId="234" priority="137" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -12305,7 +12353,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E23:F23">
+  <conditionalFormatting sqref="E25:F25">
     <cfRule type="cellIs" dxfId="231" priority="140" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -12316,7 +12364,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E23:F23">
+  <conditionalFormatting sqref="E25:F25">
     <cfRule type="cellIs" dxfId="228" priority="143" operator="equal">
       <formula>"Concluído"</formula>
     </cfRule>
@@ -12327,7 +12375,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E23:F23">
+  <conditionalFormatting sqref="E25:F25">
     <cfRule type="cellIs" dxfId="225" priority="146" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -12338,7 +12386,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E23">
+  <conditionalFormatting sqref="E25">
     <cfRule type="cellIs" dxfId="222" priority="149" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -12349,7 +12397,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E23">
+  <conditionalFormatting sqref="E25">
     <cfRule type="cellIs" dxfId="219" priority="152" operator="equal">
       <formula>"Concluído"</formula>
     </cfRule>
@@ -12360,7 +12408,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E23">
+  <conditionalFormatting sqref="E25">
     <cfRule type="cellIs" dxfId="216" priority="155" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -12371,7 +12419,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F23">
+  <conditionalFormatting sqref="F25">
     <cfRule type="cellIs" dxfId="213" priority="158" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -12382,7 +12430,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F23">
+  <conditionalFormatting sqref="F25">
     <cfRule type="cellIs" dxfId="210" priority="161" operator="equal">
       <formula>"Concluído"</formula>
     </cfRule>
@@ -12393,7 +12441,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F23">
+  <conditionalFormatting sqref="F25">
     <cfRule type="cellIs" dxfId="207" priority="164" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -12404,7 +12452,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E22:F22">
+  <conditionalFormatting sqref="E24:F24">
     <cfRule type="cellIs" dxfId="204" priority="167" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -12415,7 +12463,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E22:F22">
+  <conditionalFormatting sqref="E24:F24">
     <cfRule type="cellIs" dxfId="201" priority="170" operator="equal">
       <formula>"Concluído"</formula>
     </cfRule>
@@ -12426,7 +12474,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E22:F22">
+  <conditionalFormatting sqref="E24:F24">
     <cfRule type="cellIs" dxfId="198" priority="173" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -12437,7 +12485,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E21:F22">
+  <conditionalFormatting sqref="E23:F24">
     <cfRule type="cellIs" dxfId="195" priority="176" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -12448,7 +12496,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E21:F22">
+  <conditionalFormatting sqref="E23:F24">
     <cfRule type="cellIs" dxfId="192" priority="179" operator="equal">
       <formula>"Concluído"</formula>
     </cfRule>
@@ -12459,7 +12507,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E21:F22">
+  <conditionalFormatting sqref="E23:F24">
     <cfRule type="cellIs" dxfId="189" priority="182" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -12470,7 +12518,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E21">
+  <conditionalFormatting sqref="E23">
     <cfRule type="cellIs" dxfId="186" priority="185" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -12481,7 +12529,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E21">
+  <conditionalFormatting sqref="E23">
     <cfRule type="cellIs" dxfId="183" priority="188" operator="equal">
       <formula>"Concluído"</formula>
     </cfRule>
@@ -12492,7 +12540,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E21">
+  <conditionalFormatting sqref="E23">
     <cfRule type="cellIs" dxfId="180" priority="191" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -12503,7 +12551,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F21">
+  <conditionalFormatting sqref="F23">
     <cfRule type="cellIs" dxfId="177" priority="194" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -12514,7 +12562,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F21">
+  <conditionalFormatting sqref="F23">
     <cfRule type="cellIs" dxfId="174" priority="197" operator="equal">
       <formula>"Concluído"</formula>
     </cfRule>
@@ -12525,7 +12573,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F21">
+  <conditionalFormatting sqref="F23">
     <cfRule type="cellIs" dxfId="171" priority="200" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -12536,7 +12584,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E20:F20">
+  <conditionalFormatting sqref="E22:F22">
     <cfRule type="cellIs" dxfId="168" priority="203" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -12547,7 +12595,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E20:F20">
+  <conditionalFormatting sqref="E22:F22">
     <cfRule type="cellIs" dxfId="165" priority="206" operator="equal">
       <formula>"Concluído"</formula>
     </cfRule>
@@ -12558,7 +12606,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E20:F20">
+  <conditionalFormatting sqref="E22:F22">
     <cfRule type="cellIs" dxfId="162" priority="209" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -12569,7 +12617,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E19:F20">
+  <conditionalFormatting sqref="E21:F22">
     <cfRule type="cellIs" dxfId="159" priority="212" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -12580,7 +12628,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E19:F20">
+  <conditionalFormatting sqref="E21:F22">
     <cfRule type="cellIs" dxfId="156" priority="215" operator="equal">
       <formula>"Concluído"</formula>
     </cfRule>
@@ -12591,7 +12639,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E19:F20">
+  <conditionalFormatting sqref="E21:F22">
     <cfRule type="cellIs" dxfId="153" priority="218" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -12602,7 +12650,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E19">
+  <conditionalFormatting sqref="E21">
     <cfRule type="cellIs" dxfId="150" priority="221" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -12613,7 +12661,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E19">
+  <conditionalFormatting sqref="E21">
     <cfRule type="cellIs" dxfId="147" priority="224" operator="equal">
       <formula>"Concluído"</formula>
     </cfRule>
@@ -12624,7 +12672,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E19">
+  <conditionalFormatting sqref="E21">
     <cfRule type="cellIs" dxfId="144" priority="227" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -12635,7 +12683,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F19">
+  <conditionalFormatting sqref="F21">
     <cfRule type="cellIs" dxfId="141" priority="230" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -12646,7 +12694,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F19">
+  <conditionalFormatting sqref="F21">
     <cfRule type="cellIs" dxfId="138" priority="233" operator="equal">
       <formula>"Concluído"</formula>
     </cfRule>
@@ -12657,7 +12705,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F19">
+  <conditionalFormatting sqref="F21">
     <cfRule type="cellIs" dxfId="135" priority="236" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -12668,7 +12716,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E25 E28:F28">
+  <conditionalFormatting sqref="E27 E30:F30">
     <cfRule type="cellIs" dxfId="132" priority="239" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -12679,7 +12727,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E28:F28">
+  <conditionalFormatting sqref="E30:F30">
     <cfRule type="cellIs" dxfId="129" priority="242" operator="equal">
       <formula>"Concluído"</formula>
     </cfRule>
@@ -12690,7 +12738,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E28:F28">
+  <conditionalFormatting sqref="E30:F30">
     <cfRule type="cellIs" dxfId="126" priority="245" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -12701,7 +12749,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E27:F28">
+  <conditionalFormatting sqref="E29:F30">
     <cfRule type="cellIs" dxfId="123" priority="248" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -12712,7 +12760,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E27:F28">
+  <conditionalFormatting sqref="E29:F30">
     <cfRule type="cellIs" dxfId="120" priority="251" operator="equal">
       <formula>"Concluído"</formula>
     </cfRule>
@@ -12723,7 +12771,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E27:F28">
+  <conditionalFormatting sqref="E29:F30">
     <cfRule type="cellIs" dxfId="117" priority="254" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -12734,7 +12782,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E29:F29">
+  <conditionalFormatting sqref="E31:F31">
     <cfRule type="cellIs" dxfId="114" priority="257" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -12745,7 +12793,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E29:F29">
+  <conditionalFormatting sqref="E31:F31">
     <cfRule type="cellIs" dxfId="111" priority="260" operator="equal">
       <formula>"Concluído"</formula>
     </cfRule>
@@ -12756,7 +12804,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E29:F29">
+  <conditionalFormatting sqref="E31:F31">
     <cfRule type="cellIs" dxfId="108" priority="263" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -12767,7 +12815,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E29">
+  <conditionalFormatting sqref="E31">
     <cfRule type="cellIs" dxfId="105" priority="266" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -12778,7 +12826,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E29">
+  <conditionalFormatting sqref="E31">
     <cfRule type="cellIs" dxfId="102" priority="269" operator="equal">
       <formula>"Concluído"</formula>
     </cfRule>
@@ -12789,7 +12837,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E29">
+  <conditionalFormatting sqref="E31">
     <cfRule type="cellIs" dxfId="99" priority="272" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -12800,7 +12848,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F29">
+  <conditionalFormatting sqref="F31">
     <cfRule type="cellIs" dxfId="96" priority="275" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -12811,7 +12859,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F29">
+  <conditionalFormatting sqref="F31">
     <cfRule type="cellIs" dxfId="93" priority="278" operator="equal">
       <formula>"Concluído"</formula>
     </cfRule>
@@ -12822,7 +12870,7 @@
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F29">
+  <conditionalFormatting sqref="F31">
     <cfRule type="cellIs" dxfId="90" priority="281" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -12834,11 +12882,11 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E17:F23 E27:F29 E6:F13" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E19:F25 E29:F31 E6:F15" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"Aguardando Teste,OK,Erro,NA"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:F2 E4:F4 E15:F15 E25:F25" xr:uid="{00000000-0002-0000-0200-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:F2 E4:F4 E17:F17 E27:F27" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>"Aguardando Teste,OK,Erro,Não se Aplica"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -12873,14 +12921,14 @@
   <sheetData>
     <row r="1" spans="2:4" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="74" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
     </row>
     <row r="3" spans="2:4" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="79" t="s">
+      <c r="B3" s="82" t="s">
         <v>47</v>
       </c>
       <c r="C3" s="17" t="s">
@@ -12891,7 +12939,7 @@
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="79"/>
+      <c r="B4" s="82"/>
       <c r="C4" s="17" t="s">
         <v>50</v>
       </c>
@@ -12900,12 +12948,12 @@
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="80"/>
-      <c r="C5" s="80"/>
-      <c r="D5" s="80"/>
+      <c r="B5" s="83"/>
+      <c r="C5" s="83"/>
+      <c r="D5" s="83"/>
     </row>
     <row r="6" spans="2:4" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="79" t="s">
+      <c r="B6" s="82" t="s">
         <v>51</v>
       </c>
       <c r="C6" s="19" t="s">
@@ -12916,7 +12964,7 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B7" s="79"/>
+      <c r="B7" s="82"/>
       <c r="C7" s="19" t="s">
         <v>53</v>
       </c>
@@ -12925,7 +12973,7 @@
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="79"/>
+      <c r="B8" s="82"/>
       <c r="C8" s="19" t="s">
         <v>54</v>
       </c>
@@ -12934,7 +12982,7 @@
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="79"/>
+      <c r="B9" s="82"/>
       <c r="C9" s="19" t="s">
         <v>55</v>
       </c>
@@ -12943,7 +12991,7 @@
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="79"/>
+      <c r="B10" s="82"/>
       <c r="C10" s="19" t="s">
         <v>56</v>
       </c>
@@ -12952,7 +13000,7 @@
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="79"/>
+      <c r="B11" s="82"/>
       <c r="C11" s="19" t="s">
         <v>57</v>
       </c>
@@ -12966,7 +13014,7 @@
       <c r="D12" s="20"/>
     </row>
     <row r="13" spans="2:4" ht="23.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="77" t="s">
+      <c r="B13" s="80" t="s">
         <v>58</v>
       </c>
       <c r="C13" s="19" t="s">
@@ -12977,7 +13025,7 @@
       </c>
     </row>
     <row r="14" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B14" s="77"/>
+      <c r="B14" s="80"/>
       <c r="C14" s="19" t="s">
         <v>60</v>
       </c>
@@ -12986,7 +13034,7 @@
       </c>
     </row>
     <row r="15" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B15" s="77"/>
+      <c r="B15" s="80"/>
       <c r="C15" s="19" t="s">
         <v>61</v>
       </c>
@@ -12995,7 +13043,7 @@
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="77"/>
+      <c r="B16" s="80"/>
       <c r="C16" s="17" t="s">
         <v>62</v>
       </c>
@@ -13004,7 +13052,7 @@
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="77"/>
+      <c r="B17" s="80"/>
       <c r="C17" s="17" t="s">
         <v>63</v>
       </c>
@@ -13013,7 +13061,7 @@
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="77"/>
+      <c r="B18" s="80"/>
       <c r="C18" s="17" t="s">
         <v>62</v>
       </c>
@@ -13022,7 +13070,7 @@
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="77"/>
+      <c r="B19" s="80"/>
       <c r="C19" s="17" t="s">
         <v>63</v>
       </c>
@@ -13031,7 +13079,7 @@
       </c>
     </row>
     <row r="20" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B20" s="77"/>
+      <c r="B20" s="80"/>
       <c r="C20" s="19" t="s">
         <v>64</v>
       </c>
@@ -13045,7 +13093,7 @@
       <c r="D21" s="2"/>
     </row>
     <row r="22" spans="2:4" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="77" t="s">
+      <c r="B22" s="80" t="s">
         <v>65</v>
       </c>
       <c r="C22" s="19" t="s">
@@ -13056,7 +13104,7 @@
       </c>
     </row>
     <row r="23" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B23" s="77"/>
+      <c r="B23" s="80"/>
       <c r="C23" s="19" t="s">
         <v>67</v>
       </c>
@@ -13065,7 +13113,7 @@
       </c>
     </row>
     <row r="24" spans="2:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="77"/>
+      <c r="B24" s="80"/>
       <c r="C24" s="19" t="s">
         <v>68</v>
       </c>
@@ -13079,7 +13127,7 @@
       <c r="D25" s="2"/>
     </row>
     <row r="26" spans="2:4" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="77" t="s">
+      <c r="B26" s="80" t="s">
         <v>69</v>
       </c>
       <c r="C26" s="19" t="s">
@@ -13090,7 +13138,7 @@
       </c>
     </row>
     <row r="27" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B27" s="77"/>
+      <c r="B27" s="80"/>
       <c r="C27" s="19" t="s">
         <v>71</v>
       </c>
@@ -13099,7 +13147,7 @@
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="77"/>
+      <c r="B28" s="80"/>
       <c r="C28" s="19" t="s">
         <v>68</v>
       </c>
@@ -13112,10 +13160,10 @@
     <row r="31" spans="2:4" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="32" spans="2:4" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="33" spans="2:5" s="2" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="78" t="s">
+      <c r="B33" s="81" t="s">
         <v>72</v>
       </c>
-      <c r="C33" s="78"/>
+      <c r="C33" s="81"/>
       <c r="D33" s="21" t="s">
         <v>73</v>
       </c>
@@ -13347,14 +13395,14 @@
       <c r="D1" s="46"/>
     </row>
     <row r="2" spans="1:19" ht="18" x14ac:dyDescent="0.25">
-      <c r="B2" s="87" t="s">
+      <c r="B2" s="90" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="87"/>
-      <c r="D2" s="87"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="84" t="s">
         <v>75</v>
       </c>
       <c r="C3" s="22" t="s">
@@ -13365,7 +13413,7 @@
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B4" s="81"/>
+      <c r="B4" s="84"/>
       <c r="C4" t="s">
         <v>77</v>
       </c>
@@ -13374,7 +13422,7 @@
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="81"/>
+      <c r="B5" s="84"/>
       <c r="C5" s="23" t="s">
         <v>78</v>
       </c>
@@ -13383,7 +13431,7 @@
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B6" s="81"/>
+      <c r="B6" s="84"/>
       <c r="C6" s="23" t="s">
         <v>79</v>
       </c>
@@ -13392,12 +13440,12 @@
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B7" s="88"/>
-      <c r="C7" s="88"/>
-      <c r="D7" s="88"/>
+      <c r="B7" s="91"/>
+      <c r="C7" s="91"/>
+      <c r="D7" s="91"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B8" s="89" t="s">
+      <c r="B8" s="92" t="s">
         <v>80</v>
       </c>
       <c r="C8" s="23" t="s">
@@ -13409,7 +13457,7 @@
       <c r="E8" s="46"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="89"/>
+      <c r="B9" s="92"/>
       <c r="C9" s="23" t="s">
         <v>82</v>
       </c>
@@ -13418,7 +13466,7 @@
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="89"/>
+      <c r="B10" s="92"/>
       <c r="C10" s="23" t="s">
         <v>83</v>
       </c>
@@ -13427,7 +13475,7 @@
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="89"/>
+      <c r="B11" s="92"/>
       <c r="C11" s="23" t="s">
         <v>84</v>
       </c>
@@ -13436,7 +13484,7 @@
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B12" s="89"/>
+      <c r="B12" s="92"/>
       <c r="C12" s="23" t="s">
         <v>85</v>
       </c>
@@ -13445,7 +13493,7 @@
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B13" s="89"/>
+      <c r="B13" s="92"/>
       <c r="C13" s="23" t="s">
         <v>86</v>
       </c>
@@ -13455,9 +13503,9 @@
     </row>
     <row r="14" spans="1:19" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="24"/>
-      <c r="B14" s="90"/>
-      <c r="C14" s="90"/>
-      <c r="D14" s="90"/>
+      <c r="B14" s="93"/>
+      <c r="C14" s="93"/>
+      <c r="D14" s="93"/>
       <c r="E14" s="24"/>
       <c r="F14" s="24"/>
       <c r="G14" s="24"/>
@@ -13475,7 +13523,7 @@
       <c r="S14" s="24"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B15" s="81" t="s">
+      <c r="B15" s="84" t="s">
         <v>87</v>
       </c>
       <c r="C15" s="23" t="s">
@@ -13487,7 +13535,7 @@
       <c r="E15" s="45"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B16" s="81"/>
+      <c r="B16" s="84"/>
       <c r="C16" s="23" t="s">
         <v>89</v>
       </c>
@@ -13496,12 +13544,12 @@
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="82"/>
-      <c r="C17" s="82"/>
-      <c r="D17" s="82"/>
+      <c r="B17" s="85"/>
+      <c r="C17" s="85"/>
+      <c r="D17" s="85"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="83" t="s">
+      <c r="B18" s="86" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="64" t="s">
@@ -13512,7 +13560,7 @@
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="84"/>
+      <c r="B19" s="87"/>
       <c r="C19" s="26" t="s">
         <v>91</v>
       </c>
@@ -13527,7 +13575,7 @@
       <c r="D20" s="69"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="91" t="s">
+      <c r="B21" s="94" t="s">
         <v>92</v>
       </c>
       <c r="C21" s="59" t="s">
@@ -13538,7 +13586,7 @@
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="91"/>
+      <c r="B22" s="94"/>
       <c r="C22" s="59" t="s">
         <v>94</v>
       </c>
@@ -13547,7 +13595,7 @@
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="91"/>
+      <c r="B23" s="94"/>
       <c r="C23" s="70" t="s">
         <v>95</v>
       </c>
@@ -13571,10 +13619,10 @@
       <c r="D26" s="62"/>
     </row>
     <row r="27" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B27" s="85" t="s">
+      <c r="B27" s="88" t="s">
         <v>96</v>
       </c>
-      <c r="C27" s="86"/>
+      <c r="C27" s="89"/>
       <c r="D27" s="63" t="s">
         <v>73</v>
       </c>
@@ -13818,20 +13866,20 @@
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="2:12" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="99" t="s">
+      <c r="B3" s="102" t="s">
         <v>97</v>
       </c>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="99"/>
-      <c r="G3" s="99"/>
-      <c r="I3" s="100" t="s">
+      <c r="C3" s="102"/>
+      <c r="D3" s="102"/>
+      <c r="E3" s="102"/>
+      <c r="F3" s="102"/>
+      <c r="G3" s="102"/>
+      <c r="I3" s="103" t="s">
         <v>98</v>
       </c>
-      <c r="J3" s="100"/>
-      <c r="K3" s="100"/>
-      <c r="L3" s="100"/>
+      <c r="J3" s="103"/>
+      <c r="K3" s="103"/>
+      <c r="L3" s="103"/>
     </row>
     <row r="4" spans="2:12" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="38" t="s">
@@ -13852,13 +13900,13 @@
       <c r="G4" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="I4" s="100"/>
-      <c r="J4" s="100"/>
-      <c r="K4" s="100"/>
-      <c r="L4" s="100"/>
+      <c r="I4" s="103"/>
+      <c r="J4" s="103"/>
+      <c r="K4" s="103"/>
+      <c r="L4" s="103"/>
     </row>
     <row r="5" spans="2:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="101" t="s">
+      <c r="B5" s="104" t="s">
         <v>105</v>
       </c>
       <c r="C5" s="29" t="s">
@@ -13874,16 +13922,16 @@
         <f>IF(E5&gt;D5,0,1)</f>
         <v>0</v>
       </c>
-      <c r="G5" s="103">
+      <c r="G5" s="106">
         <v>43375</v>
       </c>
-      <c r="I5" s="100"/>
-      <c r="J5" s="100"/>
-      <c r="K5" s="100"/>
-      <c r="L5" s="100"/>
+      <c r="I5" s="103"/>
+      <c r="J5" s="103"/>
+      <c r="K5" s="103"/>
+      <c r="L5" s="103"/>
     </row>
     <row r="6" spans="2:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="101"/>
+      <c r="B6" s="104"/>
       <c r="C6" s="32" t="s">
         <v>107</v>
       </c>
@@ -13897,10 +13945,10 @@
         <f>IF(E6&gt;D6,0,1)</f>
         <v>1</v>
       </c>
-      <c r="G6" s="103"/>
+      <c r="G6" s="106"/>
     </row>
     <row r="7" spans="2:12" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="101"/>
+      <c r="B7" s="104"/>
       <c r="C7" s="32" t="s">
         <v>108</v>
       </c>
@@ -13914,16 +13962,16 @@
         <f>IF(E7&gt;D7,0,1)</f>
         <v>1</v>
       </c>
-      <c r="G7" s="103"/>
-      <c r="I7" s="105" t="s">
+      <c r="G7" s="106"/>
+      <c r="I7" s="108" t="s">
         <v>109</v>
       </c>
-      <c r="J7" s="105"/>
-      <c r="K7" s="105"/>
-      <c r="L7" s="105"/>
+      <c r="J7" s="108"/>
+      <c r="K7" s="108"/>
+      <c r="L7" s="108"/>
     </row>
     <row r="8" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="101"/>
+      <c r="B8" s="104"/>
       <c r="C8" s="32" t="s">
         <v>110</v>
       </c>
@@ -13937,14 +13985,14 @@
         <f>IF(E8&lt;D8,0,1)</f>
         <v>0</v>
       </c>
-      <c r="G8" s="103"/>
-      <c r="I8" s="105"/>
-      <c r="J8" s="105"/>
-      <c r="K8" s="105"/>
-      <c r="L8" s="105"/>
+      <c r="G8" s="106"/>
+      <c r="I8" s="108"/>
+      <c r="J8" s="108"/>
+      <c r="K8" s="108"/>
+      <c r="L8" s="108"/>
     </row>
     <row r="9" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="102"/>
+      <c r="B9" s="105"/>
       <c r="C9" s="50" t="s">
         <v>111</v>
       </c>
@@ -13958,85 +14006,85 @@
         <f>IF(E9&gt;D9,0,1)</f>
         <v>1</v>
       </c>
-      <c r="G9" s="104"/>
-      <c r="I9" s="105"/>
-      <c r="J9" s="105"/>
-      <c r="K9" s="105"/>
-      <c r="L9" s="105"/>
+      <c r="G9" s="107"/>
+      <c r="I9" s="108"/>
+      <c r="J9" s="108"/>
+      <c r="K9" s="108"/>
+      <c r="L9" s="108"/>
     </row>
     <row r="10" spans="2:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="106"/>
+      <c r="B10" s="109"/>
       <c r="C10" s="39"/>
       <c r="D10" s="40"/>
       <c r="E10" s="40"/>
       <c r="F10" s="40"/>
-      <c r="G10" s="107"/>
-      <c r="I10" s="105"/>
-      <c r="J10" s="105"/>
-      <c r="K10" s="105"/>
-      <c r="L10" s="105"/>
+      <c r="G10" s="110"/>
+      <c r="I10" s="108"/>
+      <c r="J10" s="108"/>
+      <c r="K10" s="108"/>
+      <c r="L10" s="108"/>
     </row>
     <row r="11" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="106"/>
+      <c r="B11" s="109"/>
       <c r="C11" s="39"/>
       <c r="D11" s="40"/>
       <c r="E11" s="40"/>
       <c r="F11" s="40"/>
-      <c r="G11" s="107"/>
-      <c r="I11" s="105"/>
-      <c r="J11" s="105"/>
-      <c r="K11" s="105"/>
-      <c r="L11" s="105"/>
+      <c r="G11" s="110"/>
+      <c r="I11" s="108"/>
+      <c r="J11" s="108"/>
+      <c r="K11" s="108"/>
+      <c r="L11" s="108"/>
     </row>
     <row r="12" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="106"/>
+      <c r="B12" s="109"/>
       <c r="C12" s="39"/>
       <c r="D12" s="40"/>
       <c r="E12" s="40"/>
       <c r="F12" s="40"/>
-      <c r="G12" s="107"/>
-      <c r="I12" s="105"/>
-      <c r="J12" s="105"/>
-      <c r="K12" s="105"/>
-      <c r="L12" s="105"/>
+      <c r="G12" s="110"/>
+      <c r="I12" s="108"/>
+      <c r="J12" s="108"/>
+      <c r="K12" s="108"/>
+      <c r="L12" s="108"/>
     </row>
     <row r="13" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="106"/>
+      <c r="B13" s="109"/>
       <c r="C13" s="53"/>
       <c r="D13" s="41"/>
       <c r="E13" s="41"/>
       <c r="F13" s="40"/>
-      <c r="G13" s="107"/>
-      <c r="I13" s="105"/>
-      <c r="J13" s="105"/>
-      <c r="K13" s="105"/>
-      <c r="L13" s="105"/>
+      <c r="G13" s="110"/>
+      <c r="I13" s="108"/>
+      <c r="J13" s="108"/>
+      <c r="K13" s="108"/>
+      <c r="L13" s="108"/>
     </row>
     <row r="14" spans="2:12" s="2" customFormat="1" ht="1.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="106"/>
+      <c r="B14" s="109"/>
       <c r="C14" s="39"/>
       <c r="D14" s="41"/>
       <c r="E14" s="41"/>
       <c r="F14" s="40"/>
-      <c r="G14" s="107"/>
-      <c r="I14" s="105"/>
-      <c r="J14" s="105"/>
-      <c r="K14" s="105"/>
-      <c r="L14" s="105"/>
+      <c r="G14" s="110"/>
+      <c r="I14" s="108"/>
+      <c r="J14" s="108"/>
+      <c r="K14" s="108"/>
+      <c r="L14" s="108"/>
     </row>
     <row r="15" spans="2:12" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="92" t="s">
+      <c r="B15" s="95" t="s">
         <v>112</v>
       </c>
-      <c r="C15" s="93"/>
-      <c r="D15" s="93"/>
-      <c r="E15" s="93"/>
-      <c r="F15" s="93"/>
-      <c r="G15" s="94"/>
-      <c r="I15" s="105"/>
-      <c r="J15" s="105"/>
-      <c r="K15" s="105"/>
-      <c r="L15" s="105"/>
+      <c r="C15" s="96"/>
+      <c r="D15" s="96"/>
+      <c r="E15" s="96"/>
+      <c r="F15" s="96"/>
+      <c r="G15" s="97"/>
+      <c r="I15" s="108"/>
+      <c r="J15" s="108"/>
+      <c r="K15" s="108"/>
+      <c r="L15" s="108"/>
     </row>
     <row r="16" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="56" t="s">
@@ -14057,13 +14105,13 @@
       <c r="G16" s="58" t="s">
         <v>104</v>
       </c>
-      <c r="I16" s="105"/>
-      <c r="J16" s="105"/>
-      <c r="K16" s="105"/>
-      <c r="L16" s="105"/>
+      <c r="I16" s="108"/>
+      <c r="J16" s="108"/>
+      <c r="K16" s="108"/>
+      <c r="L16" s="108"/>
     </row>
     <row r="17" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="95" t="s">
+      <c r="B17" s="98" t="s">
         <v>113</v>
       </c>
       <c r="C17" s="43" t="s">
@@ -14079,16 +14127,16 @@
         <f>IF(E17&gt;D17,0,1)</f>
         <v>0</v>
       </c>
-      <c r="G17" s="97">
+      <c r="G17" s="100">
         <v>43375</v>
       </c>
-      <c r="I17" s="105"/>
-      <c r="J17" s="105"/>
-      <c r="K17" s="105"/>
-      <c r="L17" s="105"/>
+      <c r="I17" s="108"/>
+      <c r="J17" s="108"/>
+      <c r="K17" s="108"/>
+      <c r="L17" s="108"/>
     </row>
     <row r="18" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="96"/>
+      <c r="B18" s="99"/>
       <c r="C18" s="54" t="s">
         <v>115</v>
       </c>
@@ -14102,11 +14150,11 @@
         <f>IF(E18&gt;D18,0,1)</f>
         <v>1</v>
       </c>
-      <c r="G18" s="98"/>
-      <c r="I18" s="105"/>
-      <c r="J18" s="105"/>
-      <c r="K18" s="105"/>
-      <c r="L18" s="105"/>
+      <c r="G18" s="101"/>
+      <c r="I18" s="108"/>
+      <c r="J18" s="108"/>
+      <c r="K18" s="108"/>
+      <c r="L18" s="108"/>
     </row>
     <row r="19" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="49"/>
@@ -14359,6 +14407,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100BB46273AC895BC429CDD381D3691D2B9" ma:contentTypeVersion="2" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="e1ce5b6e83737eb8f009b640c30fa88d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="35aeef18-1e63-474b-8ce4-f5abefe28d84" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8dc4da7a948ec9821969ad36af22710a" ns2:_="">
     <xsd:import namespace="35aeef18-1e63-474b-8ce4-f5abefe28d84"/>
@@ -14490,22 +14553,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B853C070-DD64-4DFA-A826-7E95875889C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A700B593-5E25-4ABB-A05F-A033C4E38350}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B5FDA3F-AA6B-418A-B72B-3C3F360D3D08}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14521,21 +14586,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A700B593-5E25-4ABB-A05F-A033C4E38350}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B853C070-DD64-4DFA-A826-7E95875889C8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>